<commit_message>
add plot næringer. One error because Haug_arbeid_raw2$desc9$region not found. Not defined by me
</commit_message>
<xml_diff>
--- a/Data/Tab_03321_andeler.xlsx
+++ b/Data/Tab_03321_andeler.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sindreespedal/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C1FA38-7FF5-6743-A158-A711D3790E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D26537-334D-9A4D-91A8-9BC580BD5656}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28760" windowHeight="17500" xr2:uid="{F47534EB-577E-DF4D-BA71-FCBA2BB6F588}"/>
   </bookViews>
@@ -601,8 +601,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C42B8E5-AE55-CF42-A31A-144E77A3E960}">
   <dimension ref="A1:J316"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView tabSelected="1" topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="F188" sqref="F188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5039,7 +5039,7 @@
         <v>51.274209989806316</v>
       </c>
       <c r="H170" s="2">
-        <v>14.028776978417264</v>
+        <v>14.18</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.2">
@@ -5065,7 +5065,7 @@
         <v>53.973843058350099</v>
       </c>
       <c r="H171" s="2">
-        <v>15.668202764976957</v>
+        <v>15.12</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.2">
@@ -5091,7 +5091,7 @@
         <v>55.381505811015664</v>
       </c>
       <c r="H172" s="2">
-        <v>14.932562620423893</v>
+        <v>15.34</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.2">
@@ -5117,7 +5117,7 @@
         <v>54.147812971342383</v>
       </c>
       <c r="H173" s="2">
-        <v>16.253443526170798</v>
+        <v>15.56</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.2">
@@ -5143,7 +5143,7 @@
         <v>55.555555555555557</v>
       </c>
       <c r="H174" s="2">
-        <v>17.460317460317459</v>
+        <v>18.22</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.2">
@@ -5169,7 +5169,7 @@
         <v>54.750479846449139</v>
       </c>
       <c r="H175" s="2">
-        <v>17.497812773403325</v>
+        <v>16.920000000000002</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.2">
@@ -5195,7 +5195,7 @@
         <v>56.399437412095644</v>
       </c>
       <c r="H176" s="2">
-        <v>20.716112531969312</v>
+        <v>18.850000000000001</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.2">
@@ -5221,7 +5221,7 @@
         <v>55.083996463306804</v>
       </c>
       <c r="H177" s="2">
-        <v>21.362229102167181</v>
+        <v>20.93</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.2">
@@ -5247,7 +5247,7 @@
         <v>53.896103896103895</v>
       </c>
       <c r="H178" s="2">
-        <v>20.581655480984338</v>
+        <v>20.64</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.2">
@@ -5273,7 +5273,7 @@
         <v>52.877542189528349</v>
       </c>
       <c r="H179" s="2">
-        <v>20.044052863436125</v>
+        <v>20.45</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.2">
@@ -5299,7 +5299,7 @@
         <v>53.586862575626625</v>
       </c>
       <c r="H180" s="2">
-        <v>20.79646017699115</v>
+        <v>19.850000000000001</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.2">
@@ -5325,7 +5325,7 @@
         <v>55.75146935348446</v>
       </c>
       <c r="H181" s="2">
-        <v>22.041420118343193</v>
+        <v>21.34</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.2">
@@ -5351,7 +5351,7 @@
         <v>56.321839080459768</v>
       </c>
       <c r="H182" s="2">
-        <v>23.287671232876711</v>
+        <v>22.17</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.2">
@@ -5377,7 +5377,7 @@
         <v>55.316558441558442</v>
       </c>
       <c r="H183" s="2">
-        <v>24.795081967213115</v>
+        <v>23.49</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.2">
@@ -5403,7 +5403,7 @@
         <v>56.768916155419227</v>
       </c>
       <c r="H184" s="2">
-        <v>26.187150837988828</v>
+        <v>25.88</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.2">
@@ -5429,7 +5429,7 @@
         <v>54.805725971370144</v>
       </c>
       <c r="H185" s="2">
-        <v>26.578073089701</v>
+        <v>26.48</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.2">
@@ -5455,7 +5455,7 @@
         <v>55.200323755564554</v>
       </c>
       <c r="H186" s="2">
-        <v>26.49402390438247</v>
+        <v>26.54</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.2">
@@ -5481,7 +5481,7 @@
         <v>56.847955537911865</v>
       </c>
       <c r="H187" s="2">
-        <v>27.046979865771814</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="188" spans="1:8" x14ac:dyDescent="0.2">
@@ -5507,7 +5507,7 @@
         <v>56.313029447357806</v>
       </c>
       <c r="H188" s="2">
-        <v>27.896138482023968</v>
+        <v>28.04</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.2">
@@ -5533,7 +5533,7 @@
         <v>57.342378292098964</v>
       </c>
       <c r="H189" s="2">
-        <v>28.542780748663098</v>
+        <v>29.06</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.2">
@@ -5559,7 +5559,7 @@
         <v>57.493956486704271</v>
       </c>
       <c r="H190" s="2">
-        <v>17.124901806755695</v>
+        <v>28.52</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>